<commit_message>
fix: update insignia spreadsheet
</commit_message>
<xml_diff>
--- a/public/norfolk-punt-sail-insignia-suffix.xlsx
+++ b/public/norfolk-punt-sail-insignia-suffix.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7880f8d83a917898/Documents/DIcks Docs/Punt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:40009_{191575AE-6676-4350-BA5D-82FFF1E4E49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00D527EA-BAC6-498D-B689-4232F48A4D07}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{10F8BA28-000F-E34E-AE37-A63CE7C693E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="norfolk-punt-register" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="138">
   <si>
     <t>Sail Number</t>
   </si>
@@ -1410,7 +1423,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1491,6 +1504,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1500,10 +1517,17 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1582,7 +1606,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F73AE41A-F6A2-497E-A4C3-FE6F4CD17B08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1612,21 +1636,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1127760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>66849</xdr:rowOff>
+      <xdr:rowOff>52561</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCB7A145-8B59-43A1-9ACC-0866EB596A34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1642,8 +1666,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3901440"/>
-          <a:ext cx="1127760" cy="981249"/>
+          <a:off x="0" y="4029077"/>
+          <a:ext cx="1127760" cy="995534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>188594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1127760</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12554</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1188720"/>
+          <a:ext cx="1127760" cy="995534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1661,9 +1734,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1701,7 +1774,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1807,7 +1880,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1949,7 +2022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1959,21 +2032,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.27734375" customWidth="1"/>
+    <col min="4" max="4" width="27.171875" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="6.72265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -1996,7 +2069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>93</v>
       </c>
@@ -2007,7 +2080,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>94</v>
       </c>
@@ -2018,7 +2091,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>95</v>
       </c>
@@ -2041,7 +2114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>95</v>
       </c>
@@ -2064,7 +2137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>95</v>
       </c>
@@ -2087,7 +2160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="76">
         <v>97</v>
@@ -2108,7 +2181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="78"/>
       <c r="B8" s="76">
         <v>95</v>
@@ -2129,7 +2202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="78"/>
       <c r="B9" s="76">
         <v>90</v>
@@ -2150,7 +2223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="78"/>
       <c r="B10" s="76">
         <v>88</v>
@@ -2171,7 +2244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="78"/>
       <c r="B11" s="76">
         <v>87</v>
@@ -2192,7 +2265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="76">
         <v>86</v>
@@ -2213,8 +2286,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="80" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="84" t="s">
         <v>95</v>
       </c>
       <c r="B13" s="76">
@@ -2236,8 +2309,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="85"/>
       <c r="B14" s="76">
         <v>82</v>
       </c>
@@ -2257,8 +2330,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="85"/>
       <c r="B15" s="76">
         <v>79</v>
       </c>
@@ -2278,8 +2351,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="85"/>
       <c r="B16" s="76">
         <v>77</v>
       </c>
@@ -2299,8 +2372,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="82"/>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="86"/>
       <c r="B17" s="77">
         <v>74</v>
       </c>
@@ -2320,7 +2393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="60" t="s">
         <v>96</v>
       </c>
@@ -2343,7 +2416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>96</v>
       </c>
@@ -2366,7 +2439,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>97</v>
       </c>
@@ -2389,7 +2462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
         <v>98</v>
       </c>
@@ -2412,9 +2485,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
-      <c r="B22" s="83">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="81"/>
+      <c r="B22" s="80">
         <v>103</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -2433,9 +2506,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="85"/>
-      <c r="B23" s="83">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="82"/>
+      <c r="B23" s="80">
         <v>102</v>
       </c>
       <c r="C23" s="29" t="s">
@@ -2454,9 +2527,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="85"/>
-      <c r="B24" s="83">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="82"/>
+      <c r="B24" s="80">
         <v>101</v>
       </c>
       <c r="C24" s="29" t="s">
@@ -2475,9 +2548,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="85"/>
-      <c r="B25" s="83">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="82"/>
+      <c r="B25" s="80">
         <v>99</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -2496,9 +2569,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="85"/>
-      <c r="B26" s="83">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="82"/>
+      <c r="B26" s="80">
         <v>98</v>
       </c>
       <c r="C26" s="29" t="s">
@@ -2517,9 +2590,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="83">
+    <row r="27" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="83"/>
+      <c r="B27" s="80">
         <v>96</v>
       </c>
       <c r="C27" s="29" t="s">
@@ -2538,11 +2611,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="80" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="83">
+      <c r="B28" s="80">
         <v>81</v>
       </c>
       <c r="C28" s="29" t="s">
@@ -2561,9 +2634,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="81"/>
-      <c r="B29" s="83">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="85"/>
+      <c r="B29" s="80">
         <v>80</v>
       </c>
       <c r="C29" s="29" t="s">
@@ -2582,9 +2655,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="81"/>
-      <c r="B30" s="83">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="85"/>
+      <c r="B30" s="80">
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
@@ -2603,9 +2676,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="81"/>
-      <c r="B31" s="83">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="85"/>
+      <c r="B31" s="80">
         <v>75</v>
       </c>
       <c r="C31" s="29" t="s">
@@ -2624,9 +2697,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="82"/>
-      <c r="B32" s="83">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="86"/>
+      <c r="B32" s="80">
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
@@ -2645,7 +2718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="61" t="s">
         <v>98</v>
       </c>
@@ -2668,7 +2741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>98</v>
       </c>
@@ -2691,7 +2764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>98</v>
       </c>
@@ -2714,7 +2787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>98</v>
       </c>
@@ -2737,7 +2810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
         <v>98</v>
       </c>
@@ -2760,7 +2833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
         <v>98</v>
       </c>
@@ -2783,7 +2856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
         <v>98</v>
       </c>
@@ -2806,7 +2879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
         <v>98</v>
       </c>
@@ -2829,7 +2902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
         <v>98</v>
       </c>
@@ -2852,7 +2925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
         <v>98</v>
       </c>
@@ -2875,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
         <v>98</v>
       </c>
@@ -2898,7 +2971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="28" t="s">
         <v>98</v>
       </c>
@@ -2921,7 +2994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
         <v>98</v>
       </c>
@@ -2944,7 +3017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="28" t="s">
         <v>98</v>
       </c>
@@ -2967,7 +3040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
         <v>98</v>
       </c>
@@ -2990,7 +3063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
         <v>98</v>
       </c>
@@ -3013,7 +3086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
         <v>98</v>
       </c>
@@ -3036,7 +3109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
         <v>98</v>
       </c>
@@ -3059,7 +3132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
         <v>98</v>
       </c>
@@ -3082,7 +3155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="28" t="s">
         <v>98</v>
       </c>
@@ -3105,7 +3178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>98</v>
       </c>
@@ -3128,7 +3201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>98</v>
       </c>
@@ -3151,49 +3224,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="54"/>
-    </row>
-    <row r="56" spans="1:7" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="16" t="s">
+      <c r="B55" s="51">
+        <v>35</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" s="51">
+        <v>893</v>
+      </c>
+      <c r="F55" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="38">
-        <v>35</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D56" s="17" t="s">
+      <c r="B56" s="43">
+        <v>30</v>
+      </c>
+      <c r="C56" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="38">
+      <c r="E56" s="43">
         <v>911</v>
       </c>
-      <c r="F56" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F56" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
         <v>100</v>
       </c>
       <c r="B57" s="43">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C57" s="44" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D57" s="44" t="s">
         <v>121</v>
@@ -3208,61 +3293,61 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="36" t="s">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="43">
-        <v>26</v>
-      </c>
-      <c r="C58" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" s="43">
+      <c r="B58" s="72">
+        <v>11</v>
+      </c>
+      <c r="C58" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" s="72">
         <v>911</v>
       </c>
-      <c r="F58" s="67" t="s">
+      <c r="F58" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="71" t="s">
+      <c r="G58" s="75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="72">
-        <v>11</v>
-      </c>
-      <c r="C59" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="E59" s="72">
+      <c r="B59" s="38">
+        <v>8</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="38">
         <v>911</v>
       </c>
-      <c r="F59" s="74" t="s">
+      <c r="F59" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G59" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>100</v>
       </c>
       <c r="B60" s="38">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>128</v>
@@ -3277,236 +3362,222 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="38">
-        <v>1</v>
-      </c>
-      <c r="C61" s="17" t="s">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="37">
         <v>89</v>
       </c>
-      <c r="D61" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E61" s="38">
-        <v>911</v>
-      </c>
-      <c r="F61" s="35" t="s">
+      <c r="C61" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E61" s="37">
+        <v>925</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="92" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="88">
+        <v>40</v>
+      </c>
+      <c r="C62" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="E62" s="88">
+        <v>926</v>
+      </c>
+      <c r="F62" s="90"/>
+      <c r="G62" s="91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="51">
+        <v>33</v>
+      </c>
+      <c r="C63" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" s="51">
+        <v>926</v>
+      </c>
+      <c r="F63" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="37">
+        <v>32</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" s="37">
+        <v>926</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="38"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="18"/>
+    </row>
+    <row r="66" spans="1:7" s="92" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="94"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="94"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="97"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="63"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="65"/>
+      <c r="G67" s="66"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="51">
+        <v>85</v>
+      </c>
+      <c r="C68" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="51">
+        <v>958</v>
+      </c>
+      <c r="F68" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G61" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="37">
-        <v>89</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E62" s="37">
-        <v>925</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="10" t="s">
+      <c r="G68" s="54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B63" s="38"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="18"/>
-    </row>
-    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="51">
-        <v>40</v>
-      </c>
-      <c r="C64" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="52" t="s">
+    <row r="69" spans="1:7" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" s="37">
+        <v>45</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" s="37">
+        <v>958</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" s="55">
+        <v>43</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" s="55">
+        <v>958</v>
+      </c>
+      <c r="F70" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="63">
+        <v>37</v>
+      </c>
+      <c r="C71" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="E64" s="51">
-        <v>944</v>
-      </c>
-      <c r="F64" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="37">
-        <v>32</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E65" s="37">
-        <v>944</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="18"/>
-    </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="B67" s="51">
-        <v>85</v>
-      </c>
-      <c r="C67" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E67" s="51">
-        <v>958</v>
-      </c>
-      <c r="F67" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="G67" s="54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="37">
-        <v>45</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E68" s="37">
-        <v>958</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" s="55">
-        <v>43</v>
-      </c>
-      <c r="C69" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D69" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" s="55">
-        <v>958</v>
-      </c>
-      <c r="F69" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="G69" s="58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B70" s="63">
-        <v>37</v>
-      </c>
-      <c r="C70" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="64" t="s">
-        <v>136</v>
-      </c>
-      <c r="E70" s="63">
+      <c r="E71" s="63">
         <v>967</v>
       </c>
-      <c r="F70" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="38">
-        <v>33</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="E71" s="38">
-        <v>967</v>
-      </c>
-      <c r="F71" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G71" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F71" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>107</v>
       </c>
@@ -3529,7 +3600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="62" t="s">
         <v>108</v>
       </c>
@@ -3552,7 +3623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
         <v>108</v>
       </c>
@@ -3575,7 +3646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
         <v>108</v>
       </c>
@@ -3598,7 +3669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="50" t="s">
         <v>109</v>
       </c>
@@ -3621,7 +3692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>109</v>
       </c>
@@ -3644,7 +3715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>109</v>
       </c>
@@ -3667,7 +3738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>109</v>
       </c>
@@ -3690,7 +3761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
         <v>110</v>
       </c>
@@ -3713,7 +3784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>111</v>
       </c>
@@ -3724,7 +3795,7 @@
       <c r="F81" s="14"/>
       <c r="G81" s="10"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
         <v>112</v>
       </c>
@@ -3747,7 +3818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="36" t="s">
         <v>112</v>
       </c>
@@ -3770,7 +3841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>113</v>
       </c>
@@ -3793,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
         <v>114</v>
       </c>
@@ -3804,7 +3875,7 @@
       <c r="F85" s="35"/>
       <c r="G85" s="18"/>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>115</v>
       </c>
@@ -3827,7 +3898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
         <v>116</v>
       </c>
@@ -3838,7 +3909,7 @@
       <c r="F87" s="35"/>
       <c r="G87" s="18"/>
     </row>
-    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>118</v>
       </c>
@@ -3861,7 +3932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
         <v>117</v>
       </c>
@@ -3881,6 +3952,7 @@
     <mergeCell ref="A28:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>